<commit_message>
added core.py and schdeule generator
</commit_message>
<xml_diff>
--- a/data/DataFile.xlsx
+++ b/data/DataFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\DS Projects\DNTProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62A1813-A1BC-4E79-BC5F-0F86C42AAD4B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464F6640-2D34-4DF4-9DC7-D9DCF77CF9CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11025" windowHeight="5625" tabRatio="617" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11025" windowHeight="5625" tabRatio="671" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prices" sheetId="6" r:id="rId1"/>
@@ -18,16 +18,23 @@
     <sheet name="Nodes" sheetId="12" r:id="rId3"/>
     <sheet name="MSoc" sheetId="13" r:id="rId4"/>
     <sheet name="Temp" sheetId="15" r:id="rId5"/>
+    <sheet name="optimun" sheetId="17" r:id="rId6"/>
+    <sheet name="solution" sheetId="18" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="Emax" localSheetId="5">#REF!</definedName>
     <definedName name="Emax" localSheetId="4">#REF!</definedName>
     <definedName name="Emax">#REF!</definedName>
+    <definedName name="energy" localSheetId="5">#REF!</definedName>
     <definedName name="energy" localSheetId="4">#REF!</definedName>
     <definedName name="energy">#REF!</definedName>
+    <definedName name="price" localSheetId="5">#REF!</definedName>
     <definedName name="price" localSheetId="4">#REF!</definedName>
     <definedName name="price">#REF!</definedName>
+    <definedName name="volume" localSheetId="5">#REF!</definedName>
     <definedName name="volume" localSheetId="4">#REF!</definedName>
     <definedName name="volume">#REF!</definedName>
+    <definedName name="weight1" localSheetId="5">#REF!</definedName>
     <definedName name="weight1" localSheetId="4">#REF!</definedName>
     <definedName name="weight1">#REF!</definedName>
   </definedNames>
@@ -41,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
   <si>
     <t>SOCmax</t>
   </si>
@@ -201,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,12 +386,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -548,11 +549,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -881,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F289"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,19 +921,19 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
         <v>3</v>
       </c>
     </row>
@@ -942,19 +941,19 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
     </row>
@@ -962,19 +961,19 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
     </row>
@@ -982,19 +981,19 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2">
-        <v>3</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
         <v>3</v>
       </c>
     </row>
@@ -1002,19 +1001,19 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2">
-        <v>3</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
     </row>
@@ -1874,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B217B0-8822-456C-9062-070D77E28C17}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,8 +1921,7 @@
         <v>13</v>
       </c>
       <c r="E3">
-        <f>D3-Nodes!D3</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2031,7 +2029,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2070,7 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2156,7 +2154,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2224,7 +2222,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E7"/>
+      <selection activeCell="D5" sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2258,38 +2256,38 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>35</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <f>B3-Nodes!B3</f>
         <v>22</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <f>C3-Nodes!C3</f>
         <v>13</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <f>D3-Nodes!D3</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>22</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <f>B4-Nodes!B4</f>
         <v>12</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <f>C4-Nodes!C4</f>
         <v>8</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <f>D4-Nodes!D4</f>
         <v>5</v>
       </c>
@@ -2298,18 +2296,18 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>40</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <f>B5-Nodes!B5</f>
         <v>37</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <f>C5-Nodes!C5</f>
         <v>31</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <f>D5-Nodes!D5</f>
         <v>27</v>
       </c>
@@ -2318,18 +2316,18 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>30</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <f>B6-Nodes!B6</f>
         <v>25</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <f>C6-Nodes!C6</f>
         <v>19</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <f>D6-Nodes!D6</f>
         <v>17</v>
       </c>
@@ -2338,20 +2336,296 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>19</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <f>B7-Nodes!B7</f>
         <v>14</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <f>C7-Nodes!C7</f>
         <v>8</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <f>D7-Nodes!D7</f>
         <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B0848A-9B75-4CDB-B794-BBCC771174D8}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>solution!B3*Prices!B3</f>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>solution!C3*Prices!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>solution!D3*Prices!D3</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>solution!E3*Prices!E3</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f>solution!B4*Prices!B4</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>solution!C4*Prices!C4</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>solution!D4*Prices!D4</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>solution!E4*Prices!E4</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f>solution!B5*Prices!B5</f>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>solution!C5*Prices!C5</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>solution!D5*Prices!D5</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>solution!E5*Prices!E5</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f>solution!B6*Prices!B6</f>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>solution!C6*Prices!C6</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>solution!D6*Prices!D6</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>solution!E6*Prices!E6</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f>solution!B7*Prices!B7</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>solution!C7*Prices!C7</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>solution!D7*Prices!D7</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>solution!E7*Prices!E7</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>SUM(B3:E7)</f>
+        <v>552</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C6DF1A-642A-44F0-9D5F-3E61AA7A43B6}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>